<commit_message>
arreglos para simulacion en excell
</commit_message>
<xml_diff>
--- a/cdc/PRUEBA DE CODIGO PUTOS DE PRUEBAS VIEJAS.xlsx
+++ b/cdc/PRUEBA DE CODIGO PUTOS DE PRUEBAS VIEJAS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WVALDOGRAELL\Documents\GitHub\RETO_I2C\Comprobacion de codigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WVALDOGRAELL\Documents\GitHub\RETO_I2C\cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632FA82F-0017-4DF9-A98D-421A22778693}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35237AF-75E7-4F63-92DD-CA12C814BB67}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28200" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,10 +174,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6170,16 +6170,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>250825</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>105410</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>153035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>177</xdr:row>
-      <xdr:rowOff>95885</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>227013</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>143510</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6467,8 +6467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H196" sqref="H196"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG137" sqref="AG137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -6487,25 +6487,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -6532,10 +6532,10 @@
       <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="7"/>
+      <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3">
@@ -6686,10 +6686,10 @@
         <f t="shared" si="3"/>
         <v>3.7024766206741333</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="7"/>
       <c r="L6">
         <v>6371</v>
       </c>

</xml_diff>